<commit_message>
Update query to get better geocode results
</commit_message>
<xml_diff>
--- a/scripts/data_v2.xlsx
+++ b/scripts/data_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\imtd-server\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445FAC9C-B2A2-4B52-A9A7-86C0EA727A2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803731B8-D8A4-4476-BEAC-5C3F925B4A91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2715" yWindow="1170" windowWidth="24990" windowHeight="13245" activeTab="1" xr2:uid="{F2A707A2-A7B0-E84A-A9D6-5519D85058CD}"/>
+    <workbookView xWindow="30000" yWindow="885" windowWidth="21225" windowHeight="12945" xr2:uid="{F2A707A2-A7B0-E84A-A9D6-5519D85058CD}"/>
   </bookViews>
   <sheets>
     <sheet name="ENTREPRISES" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="126">
   <si>
     <t>ALSTOM</t>
   </si>
@@ -358,9 +358,6 @@
     <t>LAMIH</t>
   </si>
   <si>
-    <t>fullName</t>
-  </si>
-  <si>
     <t>Laboratoire de Génie Informatique et d’Automatique de l’Artois</t>
   </si>
   <si>
@@ -412,19 +409,13 @@
     <t>Faculté des Sciences Appliquées</t>
   </si>
   <si>
-    <t>50.515735</t>
-  </si>
-  <si>
-    <t>2.655534</t>
-  </si>
-  <si>
     <t>UMR CNRS 9013</t>
   </si>
   <si>
-    <t>50.607141</t>
-  </si>
-  <si>
-    <t>3.136163</t>
+    <t>o</t>
+  </si>
+  <si>
+    <t>shortName</t>
   </si>
 </sst>
 </file>
@@ -552,7 +543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -619,6 +610,15 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -937,9 +937,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED22CB0-9506-5845-8474-5D0BC9EBCC5B}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1:N1"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -995,10 +995,10 @@
         <v>38</v>
       </c>
       <c r="M1" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="N1" s="13" t="s">
         <v>119</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
@@ -1047,7 +1047,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>8</v>
@@ -1237,15 +1237,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85B2FE07-F515-D949-B870-F9730B381209}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="26.375" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.625" style="1" customWidth="1"/>
@@ -1266,10 +1266,10 @@
         <v>82</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>106</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>94</v>
@@ -1305,10 +1305,10 @@
         <v>57</v>
       </c>
       <c r="O1" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="P1" s="13" t="s">
         <v>119</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="94.5" x14ac:dyDescent="0.25">
@@ -1325,16 +1325,16 @@
         <v>95</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="G2" s="2">
         <v>59300</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>93</v>
@@ -1358,19 +1358,19 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="G3" s="2">
         <v>62400</v>
@@ -1394,23 +1394,18 @@
         <v>77</v>
       </c>
       <c r="N3" s="2"/>
-      <c r="O3" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="P3" s="22" t="s">
-        <v>125</v>
-      </c>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
     </row>
     <row r="4" spans="1:16" ht="63" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>47</v>
@@ -1440,12 +1435,8 @@
         <v>75</v>
       </c>
       <c r="N4" s="2"/>
-      <c r="O4" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="P4" s="22" t="s">
-        <v>128</v>
-      </c>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F15" s="19"/>
@@ -1469,9 +1460,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42CF2C21-C899-EB4A-BD2B-7DA0907EFDAE}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S4" sqref="S4"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1484,12 +1475,12 @@
     <col min="7" max="7" width="18.25" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15.375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="4.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.375" style="25" customWidth="1"/>
+    <col min="11" max="11" width="8.125" style="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" style="25" customWidth="1"/>
+    <col min="13" max="13" width="11.625" style="25" customWidth="1"/>
+    <col min="14" max="14" width="15.375" style="25" customWidth="1"/>
+    <col min="15" max="15" width="5.625" style="25" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="67.375" style="1" customWidth="1"/>
     <col min="17" max="17" width="28.125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22.375" style="1" customWidth="1"/>
@@ -1501,10 +1492,10 @@
         <v>82</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>106</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>97</v>
@@ -1552,10 +1543,10 @@
         <v>57</v>
       </c>
       <c r="S1" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="T1" s="13" t="s">
         <v>119</v>
-      </c>
-      <c r="T1" s="13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="63" x14ac:dyDescent="0.25">
@@ -1563,10 +1554,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>48</v>
@@ -1578,7 +1569,7 @@
         <v>59508</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>51</v>
@@ -1586,14 +1577,24 @@
       <c r="I2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
+      <c r="J2" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="L2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+      <c r="M2" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>124</v>
+      </c>
       <c r="P2" s="2" t="s">
         <v>52</v>
       </c>
@@ -1609,6 +1610,9 @@
       <c r="B3" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>47</v>
       </c>
@@ -1617,7 +1621,7 @@
         <v>59655</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>56</v>
@@ -1625,14 +1629,24 @@
       <c r="I3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
+      <c r="J3" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="L3" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
+      <c r="M3" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="O3" s="23" t="s">
+        <v>124</v>
+      </c>
       <c r="P3" s="2" t="s">
         <v>53</v>
       </c>
@@ -1646,10 +1660,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>64</v>
@@ -1665,14 +1679,22 @@
       <c r="I4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6" t="s">
+      <c r="J4" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="L4" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6" t="s">
+      <c r="M4" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="O4" s="24" t="s">
         <v>63</v>
       </c>
       <c r="P4" s="5" t="s">

</xml_diff>